<commit_message>
add read and functionality to ExcelManager class
</commit_message>
<xml_diff>
--- a/src/main/java/com/shopwell/shopwell-inventory.xlsx
+++ b/src/main/java/com/shopwell/shopwell-inventory.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26207"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39AA8ABE-6C9B-4BA2-B133-8B973457B4D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4B0C30F-3723-4472-96B5-05BB1170E379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,36 +28,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>pName</t>
-  </si>
-  <si>
-    <t>pPrice</t>
-  </si>
-  <si>
-    <t>pQty</t>
-  </si>
-  <si>
-    <t>pCategory</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>S/No.</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Category</t>
   </si>
   <si>
     <t>Rice</t>
   </si>
   <si>
-    <t>groceries</t>
+    <t>Groceries</t>
   </si>
   <si>
     <t>Beer</t>
   </si>
   <si>
-    <t>beverages</t>
-  </si>
-  <si>
-    <t>Shirts</t>
-  </si>
-  <si>
-    <t>fashion</t>
+    <t>Drinks</t>
+  </si>
+  <si>
+    <t>Soap</t>
+  </si>
+  <si>
+    <t>Toiletries</t>
   </si>
 </sst>
 </file>
@@ -409,15 +412,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,47 +433,59 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>100</v>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
       </c>
       <c r="C2">
         <v>100</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>50</v>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
       </c>
       <c r="C3">
         <v>50</v>
       </c>
-      <c r="D3" t="s">
-        <v>7</v>
+      <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>20</v>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
       </c>
       <c r="C4">
         <v>80</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
+      <c r="D4">
+        <v>70</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed addProductToInventory and reduceProductQuantity methods in ExcelManager class
</commit_message>
<xml_diff>
--- a/src/main/java/com/shopwell/shopwell-inventory.xlsx
+++ b/src/main/java/com/shopwell/shopwell-inventory.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26207"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4B0C30F-3723-4472-96B5-05BB1170E379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FC1D14C-4249-4FB3-8E64-BF5BBA45F317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>S/No.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -51,22 +48,26 @@
     <t>Groceries</t>
   </si>
   <si>
+    <t>Jeans</t>
+  </si>
+  <si>
+    <t>Fashion</t>
+  </si>
+  <si>
+    <t>LGTV</t>
+  </si>
+  <si>
+    <t>Electronics</t>
+  </si>
+  <si>
     <t>Beer</t>
-  </si>
-  <si>
-    <t>Drinks</t>
-  </si>
-  <si>
-    <t>Soap</t>
-  </si>
-  <si>
-    <t>Toiletries</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -412,15 +413,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,59 +434,61 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="B2">
+        <v>50000</v>
+      </c>
+      <c r="C2">
+        <v>250</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>12000</v>
+      </c>
+      <c r="C3">
         <v>100</v>
       </c>
-      <c r="D2">
-        <v>100</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
+      <c r="D3" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>50</v>
-      </c>
-      <c r="D3">
-        <v>100</v>
-      </c>
-      <c r="E3" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
+      <c r="B4">
+        <v>270000</v>
       </c>
       <c r="C4">
         <v>80</v>
       </c>
-      <c r="D4">
-        <v>70</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
         <v>10</v>
+      </c>
+      <c r="B5" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactored the names of all interfaces
</commit_message>
<xml_diff>
--- a/src/main/java/com/shopwell/shopwell-inventory.xlsx
+++ b/src/main/java/com/shopwell/shopwell-inventory.xlsx
@@ -442,8 +442,8 @@
       <c r="B2">
         <v>50000</v>
       </c>
-      <c r="C2">
-        <v>250</v>
+      <c r="C2" t="n">
+        <v>230.0</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -485,7 +485,7 @@
         <v>20.0</v>
       </c>
       <c r="C5" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>

</xml_diff>